<commit_message>
Added new gear code 846, Push-up with vitjanpåse
</commit_message>
<xml_diff>
--- a/data-raw/fleet_key.xlsx
+++ b/data-raw/fleet_key.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$61</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
   <si>
     <t xml:space="preserve">metier</t>
   </si>
@@ -206,6 +209,9 @@
   </si>
   <si>
     <t xml:space="preserve">Laxfälla (Push-up)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laxfälla push up, vittjanpåse</t>
   </si>
   <si>
     <t xml:space="preserve">Laxmocka (Krona, kroksköt)</t>
@@ -313,13 +319,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -331,7 +341,21 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF2E3436"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -339,13 +363,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -943,15 +967,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>10</v>
@@ -965,7 +989,7 @@
         <v>63</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>831</v>
+        <v>843</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>10</v>
@@ -973,13 +997,16 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>832</v>
+        <v>831</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,29 +1017,29 @@
         <v>65</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>821</v>
+        <v>832</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>66</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>814</v>
+        <v>821</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>67</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>844</v>
+        <v>814</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,7 +1050,7 @@
         <v>68</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>833</v>
+        <v>844</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,16 +1061,29 @@
         <v>69</v>
       </c>
       <c r="C60" s="0" t="n">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="0" t="n">
         <v>825</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D61"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added gear code 838
</commit_message>
<xml_diff>
--- a/data-raw/fleet_key.xlsx
+++ b/data-raw/fleet_key.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$61</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$62</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="72">
   <si>
     <t xml:space="preserve">metier</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kilnot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sill-/strömmingryssja/push up, vittjanpåse</t>
   </si>
   <si>
     <t xml:space="preserve">Kombifällor (bottensatta)</t>
@@ -363,13 +366,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -914,15 +917,15 @@
         <v>812</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>10</v>
@@ -930,27 +933,27 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>828</v>
+        <v>841</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>842</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>10</v>
+        <v>828</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,35 +964,35 @@
         <v>61</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="0" t="s">
         <v>62</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>10</v>
@@ -1003,7 +1006,7 @@
         <v>64</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>831</v>
+        <v>843</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>10</v>
@@ -1011,13 +1014,16 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>832</v>
+        <v>831</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,29 +1034,29 @@
         <v>66</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>821</v>
+        <v>832</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>67</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>814</v>
+        <v>821</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>68</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>844</v>
+        <v>814</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,7 +1067,7 @@
         <v>69</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>833</v>
+        <v>844</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,11 +1078,22 @@
         <v>70</v>
       </c>
       <c r="C61" s="0" t="n">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="0" t="n">
         <v>825</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D61"/>
+  <autoFilter ref="A1:D62"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added gear code 306
</commit_message>
<xml_diff>
--- a/data-raw/fleet_key.xlsx
+++ b/data-raw/fleet_key.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$62</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$63</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t xml:space="preserve">metier</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">MIS_O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Btrål Rist, Kräfta</t>
   </si>
   <si>
     <t xml:space="preserve">Bottentrål Skarpsill</t>
@@ -366,13 +369,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="24:24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -639,7 +642,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>33</v>
       </c>
@@ -647,7 +650,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +661,7 @@
         <v>35</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,7 +672,7 @@
         <v>36</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,7 +683,7 @@
         <v>37</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -691,7 +694,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>923</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,7 +705,7 @@
         <v>39</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>327</v>
+        <v>923</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,7 +716,7 @@
         <v>40</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +727,7 @@
         <v>41</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -735,7 +738,7 @@
         <v>42</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>331</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,7 +749,7 @@
         <v>43</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>312</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,7 +760,7 @@
         <v>44</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>330</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,7 +771,7 @@
         <v>45</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>910</v>
+        <v>330</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,7 +782,7 @@
         <v>46</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>321</v>
+        <v>910</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,7 +793,7 @@
         <v>47</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,7 +804,7 @@
         <v>48</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>727</v>
+        <v>323</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +815,7 @@
         <v>49</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>311</v>
+        <v>727</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +826,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>326</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,7 +837,7 @@
         <v>51</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>725</v>
+        <v>326</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,18 +848,18 @@
         <v>52</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>53</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>714</v>
+        <v>912</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,32 +870,32 @@
         <v>54</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>822</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>10</v>
+        <v>717</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>56</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>811</v>
+        <v>822</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,10 +903,10 @@
         <v>4</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>827</v>
+        <v>811</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,35 +914,32 @@
         <v>4</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="C48" s="0" t="n">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="0" t="n">
         <v>812</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" s="0" t="n">
-        <v>838</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>10</v>
@@ -947,27 +947,27 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>828</v>
+        <v>841</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>61</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>842</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>10</v>
+        <v>828</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,35 +978,35 @@
         <v>62</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="0" t="s">
         <v>63</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>10</v>
@@ -1020,7 +1020,7 @@
         <v>65</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>831</v>
+        <v>843</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>10</v>
@@ -1028,13 +1028,16 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>66</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>832</v>
+        <v>831</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,29 +1048,29 @@
         <v>67</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>821</v>
+        <v>832</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>68</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>814</v>
+        <v>821</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>69</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>844</v>
+        <v>814</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,7 +1081,7 @@
         <v>70</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>833</v>
+        <v>844</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,11 +1092,22 @@
         <v>71</v>
       </c>
       <c r="C62" s="0" t="n">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="0" t="n">
         <v>825</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D62"/>
+  <autoFilter ref="A1:D63"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>